<commit_message>
Final change on Np
</commit_message>
<xml_diff>
--- a/input/manual_data_input.xlsx
+++ b/input/manual_data_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code_COWI\1D Solver\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5820FE-7F03-4CE4-823D-8CD59E3E93EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1C57C3-E470-4C20-97DA-5B01D1E71C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="772" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4851,7 +4851,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="128">
   <si>
     <t>layer</t>
   </si>
@@ -5318,6 +5318,9 @@
   </si>
   <si>
     <t>Jeanjean clay</t>
+  </si>
+  <si>
+    <t>Np_Jeanjean</t>
   </si>
 </sst>
 </file>
@@ -38044,8 +38047,8 @@
   </sheetPr>
   <dimension ref="A1:AT255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AT20" sqref="AT20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38088,7 +38091,9 @@
     <col min="39" max="39" width="11.7109375" style="33" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="11.5703125" style="33" bestFit="1" customWidth="1"/>
     <col min="41" max="42" width="11.5703125" style="33" customWidth="1"/>
-    <col min="43" max="16384" width="9.140625" style="33"/>
+    <col min="43" max="45" width="9.140625" style="33"/>
+    <col min="46" max="46" width="12.140625" style="33" customWidth="1"/>
+    <col min="47" max="16384" width="9.140625" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
@@ -38262,7 +38267,7 @@
         <v>123</v>
       </c>
       <c r="AT4" s="70" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:46" ht="17.25" x14ac:dyDescent="0.25">
@@ -38391,7 +38396,7 @@
         <v>109</v>
       </c>
       <c r="AT5" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
@@ -38521,7 +38526,7 @@
         <v>0.4</v>
       </c>
       <c r="AT6" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.25">
@@ -38650,7 +38655,7 @@
         <v>0.4</v>
       </c>
       <c r="AT7" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.25">
@@ -38788,7 +38793,7 @@
         <v>0.4</v>
       </c>
       <c r="AT8" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.25">
@@ -38929,7 +38934,7 @@
         <v>0.4</v>
       </c>
       <c r="AT9" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:46" s="56" customFormat="1" x14ac:dyDescent="0.25">
@@ -39070,7 +39075,7 @@
         <v>0.4</v>
       </c>
       <c r="AT10" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
@@ -39208,7 +39213,7 @@
         <v>0.2</v>
       </c>
       <c r="AT11" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
@@ -39344,7 +39349,7 @@
         <v>0.4</v>
       </c>
       <c r="AT12" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.25">
@@ -39477,7 +39482,7 @@
         <v>0.4</v>
       </c>
       <c r="AT13" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
@@ -39615,7 +39620,7 @@
         <v>0.4</v>
       </c>
       <c r="AT14" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.25">
@@ -39744,7 +39749,7 @@
         <v>0.4</v>
       </c>
       <c r="AT15" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.25">
@@ -39876,7 +39881,7 @@
         <v>0.4</v>
       </c>
       <c r="AT16" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:45" s="56" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>